<commit_message>
Added transform class and async runtime
</commit_message>
<xml_diff>
--- a/2017-03-23.xlsx
+++ b/2017-03-23.xlsx
@@ -1859,12 +1859,6 @@
       <c r="B5" t="str">
         <v>Number of DPAs at 31st March 2017</v>
       </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
       <c r="E5">
         <f>D5+C5</f>
         <v>0</v>
@@ -1874,12 +1868,6 @@
       <c r="B6" t="str">
         <v>Number of new DPAs during 01/04/16 - 31/03/17</v>
       </c>
-      <c r="C6">
-        <v>30</v>
-      </c>
-      <c r="D6">
-        <v>40</v>
-      </c>
       <c r="E6">
         <f>D6+C6</f>
         <v>0</v>
@@ -1889,12 +1877,6 @@
       <c r="B7" t="str">
         <v>Number of DPAs recovered during 01/04/16 - 31/03/17</v>
       </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-      <c r="D7">
-        <v>60</v>
-      </c>
       <c r="E7">
         <f>D7+C7</f>
         <v>0</v>
@@ -1904,12 +1886,6 @@
       <c r="B8" t="str">
         <v>Number of DPAs written off (defaulted) during 01/04/16 - 31/03/17</v>
       </c>
-      <c r="C8">
-        <v>70</v>
-      </c>
-      <c r="D8">
-        <v>80</v>
-      </c>
       <c r="E8">
         <f>D8+C8</f>
         <v>0</v>
@@ -1933,12 +1909,6 @@
       <c r="B14" t="str">
         <v>Number of DPAs at 31st March 2017</v>
       </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
       <c r="E14">
         <f>D14+C14</f>
         <v>0</v>
@@ -1948,12 +1918,6 @@
       <c r="B15" t="str">
         <v>Number of new DPAs during 01/04/16 - 31/03/17</v>
       </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
-      <c r="D15">
-        <v>40</v>
-      </c>
       <c r="E15">
         <f>D15+C15</f>
         <v>0</v>
@@ -1963,12 +1927,6 @@
       <c r="B16" t="str">
         <v>Number of DPAs recovered during 01/04/16 - 31/03/17</v>
       </c>
-      <c r="C16">
-        <v>50</v>
-      </c>
-      <c r="D16">
-        <v>60</v>
-      </c>
       <c r="E16">
         <f>D16+C16</f>
         <v>0</v>
@@ -1977,12 +1935,6 @@
     <row r="17">
       <c r="B17" t="str">
         <v>Number of DPAs written off (defaulted) during 01/04/16 - 31/03/17</v>
-      </c>
-      <c r="C17">
-        <v>70</v>
-      </c>
-      <c r="D17">
-        <v>80</v>
       </c>
       <c r="E17">
         <f>D17+C17</f>

</xml_diff>